<commit_message>
simplify thermal interview code; change the layout of code; finish e4 by question code
</commit_message>
<xml_diff>
--- a/timestamp/timestamp_zj.xlsx
+++ b/timestamp/timestamp_zj.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="177">
   <si>
     <t>Participant1</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -2241,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4051,8 +4051,8 @@
       <c r="G36" s="1">
         <v>0.48289351851851853</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>59</v>
+      <c r="H36" s="1">
+        <v>0.48298611111111112</v>
       </c>
       <c r="I36" s="1">
         <v>0.4830787037037037</v>
@@ -4100,7 +4100,7 @@
       <c r="G37" s="1">
         <v>0.49461805555555555</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="6">
         <v>0.49469907407407404</v>
       </c>
       <c r="I37" s="1">
@@ -4155,14 +4155,14 @@
       <c r="I38" s="1">
         <v>0.5128935185185185</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>59</v>
+      <c r="J38" s="1">
+        <v>0.51298611111111114</v>
       </c>
       <c r="K38" s="1">
         <v>0.51307870370370368</v>
       </c>
-      <c r="L38" s="1" t="s">
-        <v>59</v>
+      <c r="L38" s="1">
+        <v>0.5131944444444444</v>
       </c>
       <c r="M38" s="1">
         <v>0.51331018518518523</v>
@@ -4204,13 +4204,13 @@
       <c r="I39" s="1">
         <v>0.52438657407407407</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="6">
         <v>0.52447916666666672</v>
       </c>
       <c r="K39" s="1">
         <v>0.52453703703703702</v>
       </c>
-      <c r="L39" s="1">
+      <c r="L39" s="6">
         <v>0.52464120370370371</v>
       </c>
       <c r="M39" s="1">
@@ -4357,8 +4357,8 @@
       <c r="K42" s="1">
         <v>0.61259259259259258</v>
       </c>
-      <c r="L42" s="1" t="s">
-        <v>59</v>
+      <c r="L42" s="6">
+        <v>0.61280092592592594</v>
       </c>
       <c r="M42" s="1">
         <v>0.61302083333333335</v>

</xml_diff>